<commit_message>
fix a bug in FormalAmpersand
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Terms.xlsx
+++ b/AmpersandData/FormalAmpersand/Terms.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Atoms" sheetId="2" r:id="rId1"/>
-    <sheet name="Concepts" sheetId="1" r:id="rId2"/>
-    <sheet name="Relations" sheetId="3" r:id="rId3"/>
-    <sheet name="Rules" sheetId="4" r:id="rId4"/>
-    <sheet name="Terms" sheetId="5" r:id="rId5"/>
-    <sheet name="Compositions" sheetId="8" r:id="rId6"/>
-    <sheet name="Intersections" sheetId="9" r:id="rId7"/>
+    <sheet name="Concepts" sheetId="1" r:id="rId1"/>
+    <sheet name="Relations" sheetId="3" r:id="rId2"/>
+    <sheet name="Rules" sheetId="4" r:id="rId3"/>
+    <sheet name="Terms" sheetId="5" r:id="rId4"/>
+    <sheet name="Compositions" sheetId="8" r:id="rId5"/>
+    <sheet name="Intersections" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>[Concept]</t>
   </si>
@@ -34,15 +33,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>[Atom]</t>
-  </si>
-  <si>
-    <t>Atom</t>
-  </si>
-  <si>
-    <t>repr</t>
-  </si>
-  <si>
     <t>[Relation]</t>
   </si>
   <si>
@@ -53,9 +43,6 @@
   </si>
   <si>
     <t>Identifier</t>
-  </si>
-  <si>
-    <t>Representation</t>
   </si>
   <si>
     <t>A</t>
@@ -493,37 +480,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -548,7 +504,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -556,26 +512,26 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -595,30 +551,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -629,53 +585,53 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -683,64 +639,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -749,64 +705,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -829,35 +785,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -865,47 +821,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restore Atoms.adl to a demonstrable state
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Terms.xlsx
+++ b/AmpersandData/FormalAmpersand/Terms.xlsx
@@ -9,17 +9,20 @@
   <sheets>
     <sheet name="Concepts" sheetId="1" r:id="rId1"/>
     <sheet name="Relations" sheetId="3" r:id="rId2"/>
-    <sheet name="Rules" sheetId="4" r:id="rId3"/>
-    <sheet name="Terms" sheetId="5" r:id="rId4"/>
-    <sheet name="Compositions" sheetId="8" r:id="rId5"/>
-    <sheet name="Intersections" sheetId="9" r:id="rId6"/>
+    <sheet name="Rules" sheetId="12" r:id="rId3"/>
+    <sheet name="Equivalences" sheetId="10" r:id="rId4"/>
+    <sheet name="Inclusions" sheetId="4" r:id="rId5"/>
+    <sheet name="Truths" sheetId="11" r:id="rId6"/>
+    <sheet name="Terms" sheetId="5" r:id="rId7"/>
+    <sheet name="Compositions" sheetId="8" r:id="rId8"/>
+    <sheet name="Intersections" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>[Concept]</t>
   </si>
@@ -66,12 +69,6 @@
     <t>Rule</t>
   </si>
   <si>
-    <t>lhs</t>
-  </si>
-  <si>
-    <t>rhs</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>t5</t>
   </si>
   <si>
-    <t>r1</t>
-  </si>
-  <si>
     <t>[Composition]</t>
   </si>
   <si>
@@ -117,21 +111,9 @@
     <t>Intersection</t>
   </si>
   <si>
-    <t>r ISC s;t</t>
-  </si>
-  <si>
-    <t>s;t = r ISC s;t</t>
-  </si>
-  <si>
     <t>r2</t>
   </si>
   <si>
-    <t>lhTerm</t>
-  </si>
-  <si>
-    <t>rhTerm</t>
-  </si>
-  <si>
     <t>relations~</t>
   </si>
   <si>
@@ -141,7 +123,34 @@
     <t>Braga</t>
   </si>
   <si>
-    <t>rules~</t>
+    <t>[Equivalence]</t>
+  </si>
+  <si>
+    <t>Equivalence</t>
+  </si>
+  <si>
+    <t>r = s;t</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>[Inclusion]</t>
+  </si>
+  <si>
+    <t>Inclusion</t>
+  </si>
+  <si>
+    <t>[Truth]</t>
+  </si>
+  <si>
+    <t>Truth</t>
+  </si>
+  <si>
+    <t>valid</t>
   </si>
 </sst>
 </file>
@@ -554,16 +563,16 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -585,10 +594,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -602,10 +611,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -619,10 +628,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -641,128 +650,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -770,12 +684,188 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,35 +875,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -821,47 +911,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>